<commit_message>
Update compare number of filter
</commit_message>
<xml_diff>
--- a/thesis/check.xlsx
+++ b/thesis/check.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06F862E-AFAA-44B9-88F3-5BDA57FD4587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63793D0B-2AA9-44A1-A717-C532112AB873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Type of quanv" sheetId="1" r:id="rId1"/>
+    <sheet name="Diff num of quanv filter" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>mnist_4x4_quanv</t>
   </si>
@@ -39,9 +40,6 @@
     <t>Quanv</t>
   </si>
   <si>
-    <t>Not nunned</t>
-  </si>
-  <si>
     <t>Running</t>
   </si>
   <si>
@@ -61,6 +59,15 @@
   </si>
   <si>
     <t>HPC</t>
+  </si>
+  <si>
+    <t>MNIST</t>
+  </si>
+  <si>
+    <t>Number of quanv filter</t>
+  </si>
+  <si>
+    <t>Not runned</t>
   </si>
 </sst>
 </file>
@@ -410,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -459,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -476,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -493,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -518,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -532,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -546,7 +553,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -560,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -574,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -691,4 +698,191 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AFC3AE-F9F4-45F5-B80F-3F34896ACFBE}">
+  <dimension ref="A2:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.125" customWidth="1"/>
+    <col min="2" max="3" width="23.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>100</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1-100 compare number of quanv filter on mnist fashion
</commit_message>
<xml_diff>
--- a/thesis/check.xlsx
+++ b/thesis/check.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63793D0B-2AA9-44A1-A717-C532112AB873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37C480E-CB57-48EE-A4E3-8C62456A2609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>mnist_4x4_quanv</t>
   </si>
@@ -61,13 +61,16 @@
     <t>HPC</t>
   </si>
   <si>
-    <t>MNIST</t>
-  </si>
-  <si>
     <t>Number of quanv filter</t>
   </si>
   <si>
     <t>Not runned</t>
+  </si>
+  <si>
+    <t>mnist</t>
+  </si>
+  <si>
+    <t>mnist_fashion</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -702,10 +705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AFC3AE-F9F4-45F5-B80F-3F34896ACFBE}">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A4:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -714,172 +717,213 @@
     <col min="2" max="3" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
       <c r="B16" s="5">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
       <c r="B17" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>50</v>
       </c>
       <c r="B18" s="5">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>100</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="4" t="s">
-        <v>10</v>
+      <c r="C19" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update compare quanv filter
</commit_message>
<xml_diff>
--- a/thesis/check.xlsx
+++ b/thesis/check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A0401F-22B5-445A-BD3F-7567A321B82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E26801-2890-4356-A58F-B717528EB979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -175,6 +175,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -745,7 +748,7 @@
   <dimension ref="A4:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -813,8 +816,8 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="5">
-        <v>2</v>
+      <c r="B9" s="3">
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
@@ -830,11 +833,11 @@
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="2">
-        <v>2</v>
+      <c r="B10" s="3">
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -847,8 +850,8 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
-        <v>2</v>
+      <c r="B11" s="3">
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>2</v>
@@ -865,7 +868,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
@@ -893,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>7</v>
@@ -907,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
@@ -921,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>9</v>
@@ -935,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>10</v>
@@ -949,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -960,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +976,7 @@
   <dimension ref="A4:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1000,7 +1003,9 @@
       <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -1009,7 +1014,9 @@
       <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1018,7 +1025,9 @@
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1027,7 +1036,9 @@
       <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1036,7 +1047,9 @@
       <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
       <c r="F9">
         <v>0</v>
       </c>
@@ -1051,7 +1064,9 @@
       <c r="B10" s="10">
         <v>2</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="12">
+        <v>2</v>
+      </c>
       <c r="F10">
         <v>1</v>
       </c>
@@ -1064,9 +1079,11 @@
         <v>7</v>
       </c>
       <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="12">
+        <v>2</v>
+      </c>
       <c r="F11">
         <v>2</v>
       </c>
@@ -1079,18 +1096,22 @@
         <v>8</v>
       </c>
       <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2</v>
+      </c>
       <c r="F13" t="s">
         <v>6</v>
       </c>
@@ -1102,7 +1123,9 @@
       <c r="B14" s="8">
         <v>2</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="11">
+        <v>2</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1111,8 +1134,12 @@
       <c r="A15">
         <v>20</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="8">
+        <v>2</v>
+      </c>
+      <c r="C15" s="11">
+        <v>2</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1121,8 +1148,12 @@
       <c r="A16">
         <v>30</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1131,8 +1162,12 @@
       <c r="A17">
         <v>40</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="11">
+        <v>2</v>
+      </c>
       <c r="F17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1141,15 +1176,24 @@
       <c r="A18">
         <v>50</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="8">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>100</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="10">
+        <v>2</v>
+      </c>
+      <c r="C19" s="12">
+        <v>2</v>
+      </c>
+      <c r="D19" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update changed size of quanv filter
</commit_message>
<xml_diff>
--- a/thesis/check.xlsx
+++ b/thesis/check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812B392D-3861-41E8-BCE9-F394D49F1574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697A3065-751B-44D4-BDA9-F96E8E828216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1332,7 +1332,7 @@
   <dimension ref="D5:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1356,10 +1356,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1373,10 +1373,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1407,10 +1407,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.2">

</xml_diff>